<commit_message>
update analysis of false postives/negatives
</commit_message>
<xml_diff>
--- a/metric-selection/fp+fn-3/f_code+text.xlsx
+++ b/metric-selection/fp+fn-3/f_code+text.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\github\sotorrent\r-scripts\metric-selection\fp+fn-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9021D373-995D-43CE-A4E6-AD78A5848358}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-3315" windowWidth="18240" windowHeight="28440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>PostId</t>
   </si>
@@ -55,12 +54,33 @@
   </si>
   <si>
     <t>fp,fn</t>
+  </si>
+  <si>
+    <t>Semantically similar, syntactically too different</t>
+  </si>
+  <si>
+    <t>Semantically similar, syntactically too different; Should the code blocks with local ID 3 match?</t>
+  </si>
+  <si>
+    <t>Connection should be found by the metric</t>
+  </si>
+  <si>
+    <t>Connection should be found by the metric in versions 1+2, 4+5</t>
+  </si>
+  <si>
+    <t>Semantically similar, syntactically too different; Overlap should have worked in versions 4+5; Check GT in version 7+8 again</t>
+  </si>
+  <si>
+    <t>Check GT again</t>
+  </si>
+  <si>
+    <t>Semantically similar, syntactically too different; Check GT again</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -104,16 +124,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -424,14 +445,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.125" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
@@ -466,8 +487,12 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -479,7 +504,12 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -491,6 +521,12 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -502,8 +538,12 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -515,8 +555,12 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -528,7 +572,12 @@
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -540,7 +589,12 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -552,8 +606,12 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -565,8 +623,12 @@
       <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -578,8 +640,12 @@
       <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -591,8 +657,12 @@
       <c r="C12" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E13" s="2"/>
@@ -773,7 +843,7 @@
       <c r="E84" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E84" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E84"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update analysis of false positives and negatives
</commit_message>
<xml_diff>
--- a/metric-selection/fp+fn-3/f_code+text.xlsx
+++ b/metric-selection/fp+fn-3/f_code+text.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99859F0-F206-F943-8BB6-4E2900275740}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" tabRatio="500"/>
+    <workbookView xWindow="3680" yWindow="13200" windowWidth="42800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
   <si>
     <t>PostId</t>
   </si>
@@ -38,9 +39,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -75,12 +73,33 @@
   </si>
   <si>
     <t>Semantically similar, syntactically too different; Check GT again</t>
+  </si>
+  <si>
+    <t>Comment LD</t>
+  </si>
+  <si>
+    <t>Comment SB</t>
+  </si>
+  <si>
+    <t>Matching due to BELOW strategy before ABOVE strategy in combination with matched text block containing link. Can't be fixed without breaking other test cases.</t>
+  </si>
+  <si>
+    <t>Syntactically not similar enough</t>
+  </si>
+  <si>
+    <t>Fixed (now using edit-based metric if string only contain one token)</t>
+  </si>
+  <si>
+    <t>Matching strategy fails here, because semantic and syntactical similarity differ</t>
+  </si>
+  <si>
+    <t>false positive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -124,17 +143,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -445,22 +465,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9.125" customWidth="1"/>
+    <col min="1" max="3" width="9.1640625" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="51.125" customWidth="1"/>
-    <col min="6" max="1026" width="11" customWidth="1"/>
+    <col min="5" max="5" width="51.1640625" customWidth="1"/>
+    <col min="6" max="6" width="137.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="1026" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,382 +489,418 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>26578247</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>40075682</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>35161118</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>14291690</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>7016109</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>19472769</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>26578247</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>34779037</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>14159368</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>32622837</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6050383</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E14" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E33" s="2"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E49" s="2"/>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D50" s="2"/>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E54" s="2"/>
     </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
     </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
     </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E63" s="2"/>
     </row>
-    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E64" s="2"/>
     </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
     </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
     </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
     </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
     </row>
-    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
     </row>
-    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
     </row>
-    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
     </row>
-    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
     </row>
-    <row r="82" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
     </row>
-    <row r="84" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E84"/>
+  <autoFilter ref="A1:F1" xr:uid="{0DFCB1E5-72B2-384B-971E-3113FCEF1A07}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>